<commit_message>
fix calculate transitin time for route list
</commit_message>
<xml_diff>
--- a/app/data/Offprogram-good.xlsx
+++ b/app/data/Offprogram-good.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E865EF-0E1B-8F42-A4F2-599E345A71A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1277CB18-EEC0-214E-9308-9A65BE9A68C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19180" xr2:uid="{6CF93922-A14F-A84F-8887-18B6627A4F17}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{6CF93922-A14F-A84F-8887-18B6627A4F17}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
   <si>
     <t>HallName</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>авторский микс музыки «Первых романтиков» — Листа, Мендельсона, Шопена и Шумана — в исполнении DJWide и выступление Shepherd trio — одного из самых редких в мире инструментальных составов и единственных в России исполнителей музыки XVIII века для гобоев и английского рожка.</t>
+  </si>
+  <si>
+    <t>Событие</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -267,13 +270,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -282,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -628,7 +631,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,6 +717,9 @@
       <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="H3" s="7" t="b">
         <v>1</v>
       </c>
@@ -969,6 +975,9 @@
       <c r="F13" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G13" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="H13" s="7" t="b">
         <v>1</v>
       </c>
@@ -1172,6 +1181,9 @@
       <c r="F21" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G21" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="H21" s="7" t="b">
         <v>1</v>
       </c>
@@ -1191,6 +1203,9 @@
       </c>
       <c r="F22" s="6" t="s">
         <v>3</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="H22" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
ifx recomendation offprog at route list
</commit_message>
<xml_diff>
--- a/app/data/Offprogram-good.xlsx
+++ b/app/data/Offprogram-good.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1277CB18-EEC0-214E-9308-9A65BE9A68C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B53AEDF-4FDF-D44B-8EC9-72D80DE98A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{6CF93922-A14F-A84F-8887-18B6627A4F17}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -187,10 +187,10 @@
     <t>01:0:00</t>
   </si>
   <si>
-    <t>авторский микс музыки «Первых романтиков» — Листа, Мендельсона, Шопена и Шумана — в исполнении DJWide и выступление Shepherd trio — одного из самых редких в мире инструментальных составов и единственных в России исполнителей музыки XVIII века для гобоев и английского рожка.</t>
-  </si>
-  <si>
     <t>Событие</t>
+  </si>
+  <si>
+    <t>Авторский микс музыки «Первых романтиков» — Листа, Мендельсона, Шопена и Шумана — в исполнении DJWide и выступление Shepherd trio — одного из самых редких в мире инструментальных составов и единственных в России исполнителей музыки XVIII века для гобоев и английского рожка.</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8">
         <v>44743.541666666664</v>
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="7" t="b">
         <v>1</v>
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="7" t="b">
         <v>1</v>
@@ -1182,7 +1182,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H21" s="7" t="b">
         <v>1</v>
@@ -1205,7 +1205,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H22" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
fix spetial label for artists
</commit_message>
<xml_diff>
--- a/app/data/Offprogram-good.xlsx
+++ b/app/data/Offprogram-good.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B53AEDF-4FDF-D44B-8EC9-72D80DE98A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BF082E-79A5-9345-83B4-B140BD9E0C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19160" xr2:uid="{6CF93922-A14F-A84F-8887-18B6627A4F17}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t>HallName</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Музыкальный воркшоп для всей семьи</t>
-  </si>
-  <si>
-    <t>00:00:00</t>
   </si>
   <si>
     <t>Скрипка. Струнные смычковые</t>
@@ -631,7 +628,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +647,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -706,7 +703,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="8">
         <v>44743.541666666664</v>
@@ -718,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="7" t="b">
         <v>1</v>
@@ -732,7 +729,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="8">
         <v>44743.583333333336</v>
@@ -744,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="b">
         <v>1</v>
@@ -755,22 +752,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="8">
         <v>44743.625</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="7" t="b">
         <v>1</v>
@@ -784,7 +781,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8">
         <v>44743.666666666664</v>
@@ -796,7 +793,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="7" t="b">
         <v>1</v>
@@ -807,22 +804,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8">
         <v>44743.708333333336</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="7" t="b">
         <v>1</v>
@@ -833,10 +830,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D8" s="8">
         <v>44743.75</v>
@@ -848,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="7" t="b">
         <v>1</v>
@@ -886,7 +883,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="8">
         <v>44744.458333333336</v>
@@ -898,7 +895,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="7" t="b">
         <v>1</v>
@@ -909,22 +906,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="8">
         <v>44744.5</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="7" t="b">
         <v>1</v>
@@ -938,7 +935,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="8">
         <v>44744.541666666664</v>
@@ -950,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="7" t="b">
         <v>1</v>
@@ -961,10 +958,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="D13" s="8">
         <v>44744.583333333336</v>
@@ -976,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="7" t="b">
         <v>1</v>
@@ -987,22 +984,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="8">
         <v>44744.666666666664</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="7" t="b">
         <v>1</v>
@@ -1013,22 +1010,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="8">
         <v>44744.708333333336</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="7" t="b">
         <v>1</v>
@@ -1039,22 +1036,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="8">
         <v>44744.75</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="7" t="b">
         <v>1</v>
@@ -1092,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8">
         <v>44745.458333333336</v>
@@ -1104,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="7" t="b">
         <v>1</v>
@@ -1115,22 +1112,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="8">
         <v>44745.5</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="7" t="b">
         <v>1</v>
@@ -1144,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="8">
         <v>44745.541666666664</v>
@@ -1156,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="7" t="b">
         <v>1</v>
@@ -1167,22 +1164,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="D21" s="8">
         <v>44745.583333333336</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="7" t="b">
         <v>1</v>
@@ -1193,19 +1190,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="8">
         <v>44745.666666666664</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="H22" s="7" t="b">
         <v>1</v>

</xml_diff>